<commit_message>
check tushare every 5 mins until the rows for today is comes out
</commit_message>
<xml_diff>
--- a/复盘/sina/成交量M1占比.xlsx
+++ b/复盘/sina/成交量M1占比.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="47">
   <si>
     <t>date</t>
   </si>
@@ -29,6 +30,9 @@
   </si>
   <si>
     <t>0</t>
+  </si>
+  <si>
+    <t>2018-02-12</t>
   </si>
   <si>
     <t>2018-02-08</t>
@@ -158,26 +162,22 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -192,35 +192,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -508,12 +499,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
@@ -536,688 +533,708 @@
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="n">
         <v>543790.15</v>
       </c>
-      <c r="D2">
-        <v>4119.2308811</v>
-      </c>
-      <c r="E2">
-        <v>0.7575037688895248</v>
+      <c r="D2" t="n">
+        <v>3497.01666093</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.6430820162759475</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="1">
+      <c r="A3" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="n">
         <v>543790.15</v>
       </c>
-      <c r="D3">
-        <v>5265.30627268</v>
-      </c>
-      <c r="E3">
-        <v>0.9682606925998936</v>
+      <c r="D3" t="n">
+        <v>4119.2308811</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.7575037688895248</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="1">
+      <c r="A4" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="n">
         <v>543790.15</v>
       </c>
-      <c r="D4">
-        <v>5596.45308202</v>
-      </c>
-      <c r="E4">
-        <v>1.029156758727608</v>
+      <c r="D4" t="n">
+        <v>5265.30627268</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.9682606925998936</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="1">
+      <c r="A5" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="n">
         <v>543790.15</v>
       </c>
-      <c r="D5">
-        <v>4474.40115744</v>
-      </c>
-      <c r="E5">
-        <v>0.822817617685793</v>
+      <c r="D5" t="n">
+        <v>5596.45308202</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1.029156758727608</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="1">
+      <c r="A6" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="C6">
-        <v>525977.1899999999</v>
-      </c>
-      <c r="D6">
-        <v>5625.3151931</v>
-      </c>
-      <c r="E6">
-        <v>1.06949793642192</v>
+      <c r="C6" t="n">
+        <v>543790.15</v>
+      </c>
+      <c r="D6" t="n">
+        <v>4474.40115744</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.822817617685793</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="1">
+      <c r="A7" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="n">
         <v>525977.1899999999</v>
       </c>
-      <c r="D7">
-        <v>4894.08812933</v>
-      </c>
-      <c r="E7">
-        <v>0.9304753556575335</v>
+      <c r="D7" t="n">
+        <v>5625.3151931</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1.06949793642192</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="1">
+      <c r="A8" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="n">
         <v>525977.1899999999</v>
       </c>
-      <c r="D8">
-        <v>6461.49832499</v>
-      </c>
-      <c r="E8">
-        <v>1.228475007631034</v>
+      <c r="D8" t="n">
+        <v>4894.08812933</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.9304753556575335</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="1">
+      <c r="A9" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="n">
         <v>525977.1899999999</v>
       </c>
-      <c r="D9">
-        <v>4907.73112169</v>
-      </c>
-      <c r="E9">
-        <v>0.9330691929226057</v>
+      <c r="D9" t="n">
+        <v>6461.49832499</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1.228475007631034</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="1">
+      <c r="A10" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
       </c>
-      <c r="C10">
-        <v>510228.17</v>
-      </c>
-      <c r="D10">
-        <v>4973.08287541</v>
-      </c>
-      <c r="E10">
-        <v>0.974678225902345</v>
+      <c r="C10" t="n">
+        <v>525977.1899999999</v>
+      </c>
+      <c r="D10" t="n">
+        <v>4907.73112169</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.9330691929226057</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="1">
+      <c r="A11" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
       </c>
-      <c r="C11">
-        <v>496389.78</v>
-      </c>
-      <c r="D11">
-        <v>5404.961379</v>
-      </c>
-      <c r="E11">
-        <v>1.088854282817829</v>
+      <c r="C11" t="n">
+        <v>510228.17</v>
+      </c>
+      <c r="D11" t="n">
+        <v>4973.08287541</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.974678225902345</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="1">
+      <c r="A12" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B12" t="s">
         <v>15</v>
       </c>
-      <c r="C12">
-        <v>496389.78</v>
-      </c>
-      <c r="D12">
-        <v>4589.7669578</v>
-      </c>
-      <c r="E12">
-        <v>0.9246296242843677</v>
+      <c r="C12" t="n">
+        <v>496389.78</v>
+      </c>
+      <c r="D12" t="n">
+        <v>5404.961379</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1.088854282817829</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="1">
+      <c r="A13" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B13" t="s">
         <v>16</v>
       </c>
-      <c r="C13">
-        <v>496389.78</v>
-      </c>
-      <c r="D13">
-        <v>5524.87386658</v>
-      </c>
-      <c r="E13">
-        <v>1.113011203933328</v>
+      <c r="C13" t="n">
+        <v>496389.78</v>
+      </c>
+      <c r="D13" t="n">
+        <v>4589.7669578</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.9246296242843677</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="1">
+      <c r="A14" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B14" t="s">
         <v>17</v>
       </c>
-      <c r="C14">
-        <v>496389.78</v>
-      </c>
-      <c r="D14">
-        <v>4606.85651392</v>
-      </c>
-      <c r="E14">
-        <v>0.9280723938192281</v>
+      <c r="C14" t="n">
+        <v>496389.78</v>
+      </c>
+      <c r="D14" t="n">
+        <v>5524.87386658</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1.113011203933328</v>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="1">
+      <c r="A15" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B15" t="s">
         <v>18</v>
       </c>
-      <c r="C15">
-        <v>496389.78</v>
-      </c>
-      <c r="D15">
-        <v>4342.43604047</v>
-      </c>
-      <c r="E15">
-        <v>0.8748036755450525</v>
+      <c r="C15" t="n">
+        <v>496389.78</v>
+      </c>
+      <c r="D15" t="n">
+        <v>4606.85651392</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.9280723938192281</v>
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="1">
+      <c r="A16" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B16" t="s">
         <v>19</v>
       </c>
-      <c r="C16">
-        <v>496389.78</v>
-      </c>
-      <c r="D16">
-        <v>5245.97054928</v>
-      </c>
-      <c r="E16">
-        <v>1.056824850277941</v>
+      <c r="C16" t="n">
+        <v>496389.78</v>
+      </c>
+      <c r="D16" t="n">
+        <v>4342.43604047</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.8748036755450525</v>
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="1">
+      <c r="A17" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B17" t="s">
         <v>20</v>
       </c>
-      <c r="C17">
-        <v>496389.78</v>
-      </c>
-      <c r="D17">
-        <v>4485.45211229</v>
-      </c>
-      <c r="E17">
-        <v>0.9036149197692989</v>
+      <c r="C17" t="n">
+        <v>496389.78</v>
+      </c>
+      <c r="D17" t="n">
+        <v>5245.97054928</v>
+      </c>
+      <c r="E17" t="n">
+        <v>1.056824850277941</v>
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="1">
+      <c r="A18" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B18" t="s">
         <v>21</v>
       </c>
-      <c r="C18">
-        <v>496389.78</v>
-      </c>
-      <c r="D18">
-        <v>5007.75223648</v>
-      </c>
-      <c r="E18">
-        <v>1.008834677555207</v>
+      <c r="C18" t="n">
+        <v>496389.78</v>
+      </c>
+      <c r="D18" t="n">
+        <v>4485.45211229</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.9036149197692989</v>
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="1">
+      <c r="A19" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B19" t="s">
         <v>22</v>
       </c>
-      <c r="C19">
-        <v>496389.78</v>
-      </c>
-      <c r="D19">
-        <v>4663.16876628</v>
-      </c>
-      <c r="E19">
-        <v>0.9394167555746212</v>
+      <c r="C19" t="n">
+        <v>496389.78</v>
+      </c>
+      <c r="D19" t="n">
+        <v>5007.75223648</v>
+      </c>
+      <c r="E19" t="n">
+        <v>1.008834677555207</v>
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="1">
+      <c r="A20" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B20" t="s">
         <v>23</v>
       </c>
-      <c r="C20">
-        <v>496389.78</v>
-      </c>
-      <c r="D20">
-        <v>4763.88038986</v>
-      </c>
-      <c r="E20">
-        <v>0.9597055744902725</v>
+      <c r="C20" t="n">
+        <v>496389.78</v>
+      </c>
+      <c r="D20" t="n">
+        <v>4663.16876628</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.9394167555746212</v>
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="1">
+      <c r="A21" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B21" t="s">
         <v>24</v>
       </c>
-      <c r="C21">
-        <v>496389.78</v>
-      </c>
-      <c r="D21">
-        <v>4099.2806756</v>
-      </c>
-      <c r="E21">
-        <v>0.8258189110178699</v>
+      <c r="C21" t="n">
+        <v>496389.78</v>
+      </c>
+      <c r="D21" t="n">
+        <v>4763.88038986</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.9597055744902725</v>
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="1">
+      <c r="A22" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B22" t="s">
         <v>25</v>
       </c>
-      <c r="C22">
-        <v>496389.78</v>
-      </c>
-      <c r="D22">
-        <v>3840.27186082</v>
-      </c>
-      <c r="E22">
-        <v>0.7736403962265298</v>
+      <c r="C22" t="n">
+        <v>496389.78</v>
+      </c>
+      <c r="D22" t="n">
+        <v>4099.2806756</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.8258189110178699</v>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="1">
+      <c r="A23" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B23" t="s">
         <v>26</v>
       </c>
-      <c r="C23">
-        <v>496389.78</v>
-      </c>
-      <c r="D23">
-        <v>3379.00285005</v>
-      </c>
-      <c r="E23">
-        <v>0.6807156364198311</v>
+      <c r="C23" t="n">
+        <v>496389.78</v>
+      </c>
+      <c r="D23" t="n">
+        <v>3840.27186082</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.7736403962265298</v>
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="1">
+      <c r="A24" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B24" t="s">
         <v>27</v>
       </c>
-      <c r="C24">
-        <v>496389.78</v>
-      </c>
-      <c r="D24">
-        <v>3515.05383076</v>
-      </c>
-      <c r="E24">
-        <v>0.708123731064729</v>
+      <c r="C24" t="n">
+        <v>496389.78</v>
+      </c>
+      <c r="D24" t="n">
+        <v>3379.00285005</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.6807156364198311</v>
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="1">
+      <c r="A25" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B25" t="s">
         <v>28</v>
       </c>
-      <c r="C25">
-        <v>496389.78</v>
-      </c>
-      <c r="D25">
-        <v>3716.7509126</v>
-      </c>
-      <c r="E25">
-        <v>0.7487565341494339</v>
+      <c r="C25" t="n">
+        <v>496389.78</v>
+      </c>
+      <c r="D25" t="n">
+        <v>3515.05383076</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.708123731064729</v>
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="1">
+      <c r="A26" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B26" t="s">
         <v>29</v>
       </c>
-      <c r="C26">
-        <v>496389.78</v>
-      </c>
-      <c r="D26">
-        <v>3829.32336726</v>
-      </c>
-      <c r="E26">
-        <v>0.7714347719366825</v>
+      <c r="C26" t="n">
+        <v>496389.78</v>
+      </c>
+      <c r="D26" t="n">
+        <v>3716.7509126</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.7487565341494339</v>
       </c>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="1">
+      <c r="A27" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B27" t="s">
         <v>30</v>
       </c>
-      <c r="C27">
-        <v>496389.78</v>
-      </c>
-      <c r="D27">
-        <v>4392.65140698</v>
-      </c>
-      <c r="E27">
-        <v>0.8849197916564679</v>
+      <c r="C27" t="n">
+        <v>496389.78</v>
+      </c>
+      <c r="D27" t="n">
+        <v>3829.32336726</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.7714347719366825</v>
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="1">
+      <c r="A28" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B28" t="s">
         <v>31</v>
       </c>
-      <c r="C28">
-        <v>496389.78</v>
-      </c>
-      <c r="D28">
-        <v>4053.97266986</v>
-      </c>
-      <c r="E28">
-        <v>0.8166914052622114</v>
+      <c r="C28" t="n">
+        <v>496389.78</v>
+      </c>
+      <c r="D28" t="n">
+        <v>4392.65140698</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.8849197916564679</v>
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="1">
+      <c r="A29" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B29" t="s">
         <v>32</v>
       </c>
-      <c r="C29">
-        <v>496389.78</v>
-      </c>
-      <c r="D29">
-        <v>4780.73652266</v>
-      </c>
-      <c r="E29">
-        <v>0.9631013198257224</v>
+      <c r="C29" t="n">
+        <v>496389.78</v>
+      </c>
+      <c r="D29" t="n">
+        <v>4053.97266986</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.8166914052622114</v>
       </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="1">
+      <c r="A30" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B30" t="s">
         <v>33</v>
       </c>
-      <c r="C30">
-        <v>496389.78</v>
-      </c>
-      <c r="D30">
-        <v>3922.23703732</v>
-      </c>
-      <c r="E30">
-        <v>0.7901526573169979</v>
+      <c r="C30" t="n">
+        <v>496389.78</v>
+      </c>
+      <c r="D30" t="n">
+        <v>4780.73652266</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.9631013198257224</v>
       </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="1">
+      <c r="A31" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B31" t="s">
         <v>34</v>
       </c>
-      <c r="C31">
-        <v>496389.78</v>
-      </c>
-      <c r="D31">
-        <v>3982.54604492</v>
-      </c>
-      <c r="E31">
-        <v>0.802302183763735</v>
+      <c r="C31" t="n">
+        <v>496389.78</v>
+      </c>
+      <c r="D31" t="n">
+        <v>3922.23703732</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.7901526573169979</v>
       </c>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="1">
+      <c r="A32" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B32" t="s">
         <v>35</v>
       </c>
-      <c r="C32">
-        <v>490180.42</v>
-      </c>
-      <c r="D32">
-        <v>3509.86621306</v>
-      </c>
-      <c r="E32">
-        <v>0.7160355799319769</v>
+      <c r="C32" t="n">
+        <v>496389.78</v>
+      </c>
+      <c r="D32" t="n">
+        <v>3982.54604492</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.802302183763735</v>
       </c>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="1">
+      <c r="A33" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B33" t="s">
         <v>36</v>
       </c>
-      <c r="C33">
+      <c r="C33" t="n">
         <v>490180.42</v>
       </c>
-      <c r="D33">
-        <v>3632.39468145</v>
-      </c>
-      <c r="E33">
-        <v>0.7410321859551224</v>
+      <c r="D33" t="n">
+        <v>3509.86621306</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.7160355799319769</v>
       </c>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="1">
+      <c r="A34" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B34" t="s">
         <v>37</v>
       </c>
-      <c r="C34">
+      <c r="C34" t="n">
         <v>490180.42</v>
       </c>
-      <c r="D34">
-        <v>4130.88275483</v>
-      </c>
-      <c r="E34">
-        <v>0.8427270013824706</v>
+      <c r="D34" t="n">
+        <v>3632.39468145</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.7410321859551224</v>
       </c>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="1">
+      <c r="A35" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B35" t="s">
         <v>38</v>
       </c>
-      <c r="C35">
+      <c r="C35" t="n">
         <v>490180.42</v>
       </c>
-      <c r="D35">
-        <v>3824.81972962</v>
-      </c>
-      <c r="E35">
-        <v>0.7802881497429049</v>
+      <c r="D35" t="n">
+        <v>4130.88275483</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.8427270013824706</v>
       </c>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" s="1">
+      <c r="A36" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B36" t="s">
         <v>39</v>
       </c>
-      <c r="C36">
+      <c r="C36" t="n">
         <v>490180.42</v>
       </c>
-      <c r="D36">
-        <v>3570.71200243</v>
-      </c>
-      <c r="E36">
-        <v>0.7284485174724034</v>
+      <c r="D36" t="n">
+        <v>3824.81972962</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.7802881497429049</v>
       </c>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="1">
+      <c r="A37" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B37" t="s">
         <v>40</v>
       </c>
-      <c r="C37">
+      <c r="C37" t="n">
         <v>490180.42</v>
       </c>
-      <c r="D37">
-        <v>3872.77760594</v>
-      </c>
-      <c r="E37">
-        <v>0.790071869035487</v>
+      <c r="D37" t="n">
+        <v>3570.71200243</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0.7284485174724034</v>
       </c>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="1">
+      <c r="A38" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B38" t="s">
         <v>41</v>
       </c>
-      <c r="C38">
+      <c r="C38" t="n">
         <v>490180.42</v>
       </c>
-      <c r="D38">
-        <v>4265.00352376</v>
-      </c>
-      <c r="E38">
-        <v>0.8700885122584048</v>
+      <c r="D38" t="n">
+        <v>3872.77760594</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.790071869035487</v>
       </c>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="1">
+      <c r="A39" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B39" t="s">
         <v>42</v>
       </c>
-      <c r="C39">
+      <c r="C39" t="n">
         <v>490180.42</v>
       </c>
-      <c r="D39">
-        <v>4558.16716123</v>
-      </c>
-      <c r="E39">
-        <v>0.9298958047385899</v>
+      <c r="D39" t="n">
+        <v>4265.00352376</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.8700885122584048</v>
       </c>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="1">
+      <c r="A40" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B40" t="s">
         <v>43</v>
       </c>
-      <c r="C40">
+      <c r="C40" t="n">
         <v>490180.42</v>
       </c>
-      <c r="D40">
-        <v>2978.21369346</v>
-      </c>
-      <c r="E40">
-        <v>0.6075750013556233</v>
+      <c r="D40" t="n">
+        <v>4558.16716123</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.9298958047385899</v>
       </c>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="1">
+      <c r="A41" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B41" t="s">
         <v>44</v>
       </c>
-      <c r="C41">
+      <c r="C41" t="n">
         <v>490180.42</v>
       </c>
-      <c r="D41">
-        <v>3219.62642126</v>
-      </c>
-      <c r="E41">
-        <v>0.6568247710220658</v>
+      <c r="D41" t="n">
+        <v>2978.21369346</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.6075750013556233</v>
       </c>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="1">
+      <c r="A42" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B42" t="s">
         <v>45</v>
       </c>
+      <c r="C42" t="n">
+        <v>490180.42</v>
+      </c>
+      <c r="D42" t="n">
+        <v>3219.62642126</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.6568247710220658</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B43" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43" t="s"/>
+      <c r="D43" t="s"/>
+      <c r="E43" t="s"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>